<commit_message>
Added Scorpions VDMS. PAS-1487 Update year in specified VIN after premium Calc
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VINupload_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VINupload_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +673,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="3">
-        <v>2017</v>
+        <v>2005</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -805,5 +805,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>